<commit_message>
Added Roman to integer problem solution
</commit_message>
<xml_diff>
--- a/Python/Solutions_Addendum.xlsx
+++ b/Python/Solutions_Addendum.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nagasudheerravela/Desktop/Interview_Kickstart/Leetcode_PythonSols/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304BE6C0-5463-A444-B92B-6A94FFFA3FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDC85E9-A0F2-B244-8BDC-03E8443F237F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D384EB79-E46B-E34E-B624-6E4E8F264DD9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{D384EB79-E46B-E34E-B624-6E4E8F264DD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">Problem </t>
   </si>
@@ -91,12 +91,65 @@
   <si>
     <t xml:space="preserve">1.List </t>
   </si>
+  <si>
+    <t>Meeting Rooms II</t>
+  </si>
+  <si>
+    <r>
+      <t>Input:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF263238"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> intervals = [[0,30],[5,10],[15,20]]</t>
+    </r>
+  </si>
+  <si>
+    <t>Output: 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Think through this problem in real
+time scenerio. We need to provide meeting rooms to one team whose start time is much earlier and ask them to leave once end time completes
+Min heap can be used in this case_x000B__x000B_1.first sort all intervals by start time
+2.push first interval into min heap 
+[0,30]
+3.for next interval , retrieve min_heap[0][-1] which is end time of fast available
+heap and compare end time of interval to it.  
+min_heap = [[0,30]]
+interval  = [5,10]
+30 &gt; 5 which means it needs a seperate room 
+so push it to heap 
+4.for intervals which have end time &gt; min_heap[0][-1] . we can pop it and give that room to new interval 
+min_heap = [[5,10],[0,30]]
+interva = [15,20]
+10 &lt; 15
+so pop min_heap
+and push new interval
+ </t>
+  </si>
+  <si>
+    <t>Time Complexity: O(N\log N)O(NlogN).
+There are two major portions that take up time here. One is sorting of the array that takes O(N\log N)O(NlogN) considering that the array consists of NN elements.
+Then we have the min-heap. In the worst case, all NN meetings will collide with each other. In any case we have NN add operations on the heap. In the worst case we will have NN extract-min operations as well. Overall complexity being (NlogN)(NlogN) since extract-min operation on a heap takes O(\log N)O(logN).
+Space Complexity: O(N)O(N) because we construct the min-heap and that can contain NN elements in the worst case as described above in the time complexity section. Hence, the space complexity is O(N)O(N).</t>
+  </si>
+  <si>
+    <t>min_heap</t>
+  </si>
+  <si>
+    <t>3Sum</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -113,6 +166,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color rgb="FF263238"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF212121"/>
+      <name val="PingFang SC"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color rgb="FF263238"/>
       <name val="Consolas"/>
@@ -140,13 +207,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -462,13 +531,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6F96BD-FC68-7545-8D31-A286409A3E58}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="36.83203125" customWidth="1"/>
     <col min="3" max="3" width="62.6640625" customWidth="1"/>
@@ -477,7 +546,7 @@
     <col min="6" max="6" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -500,7 +569,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="313" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="313" customHeight="1">
       <c r="A2">
         <v>56</v>
       </c>
@@ -523,10 +592,42 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="202" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:7" ht="313" customHeight="1">
+      <c r="A3" s="4">
+        <v>253</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="24">
+      <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="5"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{422DC4F6-CC54-BA49-8E19-6B727433D272}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{3B7CE275-DFEC-454E-909F-4F9A7C70A73E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
242 Valid Anagram solution
</commit_message>
<xml_diff>
--- a/Python/Solutions_Addendum.xlsx
+++ b/Python/Solutions_Addendum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nagasudheerravela/Desktop/Interview_Kickstart/Leetcode_PythonSols/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDC85E9-A0F2-B244-8BDC-03E8443F237F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E28CFE2-9D48-0642-BBEA-0C0DB62111DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{D384EB79-E46B-E34E-B624-6E4E8F264DD9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t xml:space="preserve">Problem </t>
   </si>
@@ -142,14 +142,72 @@
     <t>min_heap</t>
   </si>
   <si>
-    <t>3Sum</t>
+    <t>Contains Duplicate</t>
+  </si>
+  <si>
+    <t>Input: nums = [1,2,3,1]</t>
+  </si>
+  <si>
+    <r>
+      <t>Output:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF263238"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> true</t>
+    </r>
+  </si>
+  <si>
+    <t>For Finding Duplicate items in a unsorted list .we can solve it in 2 ways 
+1. Presorting O(nlogn)+search if adjacent elements are equal
+2. create a hasmap/set to capture elements and see if it already excists in list return duplicate  O(n)</t>
+  </si>
+  <si>
+    <t>hashmap</t>
+  </si>
+  <si>
+    <t>set
+hashmap</t>
+  </si>
+  <si>
+    <t>Valid Anagram</t>
+  </si>
+  <si>
+    <r>
+      <t>Input:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF263238"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> s = "anagram", t = "nagaram"</t>
+    </r>
+  </si>
+  <si>
+    <t>sol-1
+        build hashmap for both strings to capture characters and their counts
+        if both hashmaps are equal then return true else false
+        part-1 O(N) -&gt; for building hashmap
+        part-2 O(N) for comparing counts in both hashmaps
+        Space complexity -&gt; 2 O(n)
+sol-2
+        1. create hashmap and will doing it use single hashmap to increment and decrement counts
+        2. each value in final dictionary should be 0  
+        Space complexity -&gt;  O(n)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -172,18 +230,31 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="16"/>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF263238"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF212121"/>
       <name val="PingFang SC"/>
       <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color rgb="FF263238"/>
-      <name val="Consolas"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF212121"/>
+      <name val="PingFang SC"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -207,7 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -215,7 +286,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -531,14 +605,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6F96BD-FC68-7545-8D31-A286409A3E58}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="1" width="10.83203125" style="5"/>
     <col min="2" max="2" width="36.83203125" customWidth="1"/>
     <col min="3" max="3" width="62.6640625" customWidth="1"/>
     <col min="4" max="4" width="29.1640625" customWidth="1"/>
@@ -547,7 +622,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B1" t="s">
@@ -570,7 +645,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="313" customHeight="1">
-      <c r="A2">
+      <c r="A2" s="5">
         <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -593,13 +668,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="313" customHeight="1">
-      <c r="A3" s="4">
+      <c r="A3" s="6">
         <v>253</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
@@ -615,19 +690,52 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="24">
-      <c r="A4">
-        <v>15</v>
-      </c>
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:7" ht="147" customHeight="1">
+      <c r="A4" s="7">
+        <v>217</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="224">
+      <c r="A5" s="8">
+        <v>242</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{422DC4F6-CC54-BA49-8E19-6B727433D272}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{3B7CE275-DFEC-454E-909F-4F9A7C70A73E}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{CB7F32F9-7BF2-AC4D-B5A1-1706D1FC7A71}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{7ACC022D-9E8F-1340-BB6C-E100B9999DBF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
242 Valid Anagram solution (2 other solutions)
</commit_message>
<xml_diff>
--- a/Python/Solutions_Addendum.xlsx
+++ b/Python/Solutions_Addendum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nagasudheerravela/Desktop/Interview_Kickstart/Leetcode_PythonSols/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E28CFE2-9D48-0642-BBEA-0C0DB62111DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE98101-AEBC-004B-824D-845DB5FB5A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{D384EB79-E46B-E34E-B624-6E4E8F264DD9}"/>
   </bookViews>
@@ -167,9 +167,6 @@
 2. create a hasmap/set to capture elements and see if it already excists in list return duplicate  O(n)</t>
   </si>
   <si>
-    <t>hashmap</t>
-  </si>
-  <si>
     <t>set
 hashmap</t>
   </si>
@@ -200,7 +197,15 @@
 sol-2
         1. create hashmap and will doing it use single hashmap to increment and decrement counts
         2. each value in final dictionary should be 0  
-        Space complexity -&gt;  O(n)</t>
+        Space complexity -&gt;  O(n)
+sol3
+    1.presorting and compare
+sol4
+    1. Preallocate 2 lists with size of 26 (all alphabets)-each index is for one alphabet
+	2. increment alphabet if elem is in s, decrement if it is in t</t>
+  </si>
+  <si>
+    <t>hashmap,list[aphabets]</t>
   </si>
 </sst>
 </file>
@@ -608,7 +613,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -619,6 +624,7 @@
     <col min="4" max="4" width="29.1640625" customWidth="1"/>
     <col min="5" max="5" width="67.5" customWidth="1"/>
     <col min="6" max="6" width="31.5" customWidth="1"/>
+    <col min="7" max="7" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -707,27 +713,27 @@
         <v>22</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="224">
+    <row r="5" spans="1:7" ht="359">
       <c r="A5" s="8">
         <v>242</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
         <v>27</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated comment to 1.Two Sum problem
</commit_message>
<xml_diff>
--- a/Python/Solutions_Addendum.xlsx
+++ b/Python/Solutions_Addendum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nagasudheerravela/Desktop/Interview_Kickstart/Leetcode_PythonSols/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE98101-AEBC-004B-824D-845DB5FB5A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA249478-0F3F-1E46-B030-37C500576B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{D384EB79-E46B-E34E-B624-6E4E8F264DD9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t xml:space="preserve">Problem </t>
   </si>
@@ -206,6 +206,36 @@
   </si>
   <si>
     <t>hashmap,list[aphabets]</t>
+  </si>
+  <si>
+    <t>Two Sum</t>
+  </si>
+  <si>
+    <r>
+      <t>Input:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF263238"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> nums = [2,7,11,15], target = 9</t>
+    </r>
+  </si>
+  <si>
+    <t>Output: [0,1]
+Explanation: Because nums[0] + nums[1] == 9, we return [0, 1].</t>
+  </si>
+  <si>
+    <t>hasmap</t>
+  </si>
+  <si>
+    <t>push elem and index into dictionary and if target-elem is already in it return index of elem and target-elem</t>
+  </si>
+  <si>
+    <t>O(n) , O(n)-Time and space complexity</t>
   </si>
 </sst>
 </file>
@@ -610,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6F96BD-FC68-7545-8D31-A286409A3E58}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -736,12 +766,36 @@
         <v>27</v>
       </c>
     </row>
+    <row r="6" spans="1:7" ht="51">
+      <c r="A6" s="5">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{422DC4F6-CC54-BA49-8E19-6B727433D272}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{3B7CE275-DFEC-454E-909F-4F9A7C70A73E}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{CB7F32F9-7BF2-AC4D-B5A1-1706D1FC7A71}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{7ACC022D-9E8F-1340-BB6C-E100B9999DBF}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{CCADE891-1C52-6E4B-856F-E2835475C144}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added List in Basics and 1.Two Sum 49.Group Anagrams 347.Top K Frequent Elements
</commit_message>
<xml_diff>
--- a/Python/Solutions_Addendum.xlsx
+++ b/Python/Solutions_Addendum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nagasudheerravela/Desktop/Interview_Kickstart/Leetcode_PythonSols/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA249478-0F3F-1E46-B030-37C500576B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB416573-717C-5E46-9445-E0E77EA0902F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{D384EB79-E46B-E34E-B624-6E4E8F264DD9}"/>
   </bookViews>
@@ -643,7 +643,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>